<commit_message>
Re-added 0402 capacitor part#to the BOM
Signed-off-by: Marcos Chaparro <marcos@mrkindustries.com.ar>
</commit_message>
<xml_diff>
--- a/design/BLDC4.5_BOM.xlsx
+++ b/design/BLDC4.5_BOM.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="571" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Tabell1" state="visible" r:id="rId3"/>
+    <sheet name="Tabell1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="188">
   <si>
     <t>MFG Part# (digikey)</t>
   </si>
@@ -43,10 +47,10 @@
     <t>U1</t>
   </si>
   <si>
-    <t>SPX1117M3-L-3-3 </t>
-  </si>
-  <si>
-    <t>701-SPX1117M3-L-3-3 </t>
+    <t>SPX1117M3-L-3-3</t>
+  </si>
+  <si>
+    <t>701-SPX1117M3-L-3-3</t>
   </si>
   <si>
     <t>VREG</t>
@@ -73,7 +77,7 @@
     <t>SN65HVD232DR</t>
   </si>
   <si>
-    <t> 595-SN65HVD232DR</t>
+    <t>595-SN65HVD232DR</t>
   </si>
   <si>
     <t>CAN Transceiver</t>
@@ -85,7 +89,7 @@
     <t>LM73CIMK-0/NOPB</t>
   </si>
   <si>
-    <t> 926-LM73CIMK-0/NOPB</t>
+    <t>926-LM73CIMK-0/NOPB</t>
   </si>
   <si>
     <t>Temp sensor</t>
@@ -106,10 +110,10 @@
     <t>L1</t>
   </si>
   <si>
-    <t>UX60R-MB-5ST </t>
-  </si>
-  <si>
-    <t> 798-UX60R-MB-5ST </t>
+    <t>UX60R-MB-5ST</t>
+  </si>
+  <si>
+    <t>798-UX60R-MB-5ST</t>
   </si>
   <si>
     <t>Mini-USB</t>
@@ -130,10 +134,10 @@
     <t>X2</t>
   </si>
   <si>
-    <t>IRFS3006-7PPBF </t>
-  </si>
-  <si>
-    <t>942-IRFS3006-7PPBF </t>
+    <t>IRFS3006-7PPBF</t>
+  </si>
+  <si>
+    <t>942-IRFS3006-7PPBF</t>
   </si>
   <si>
     <t>MOSFET 60V 240A</t>
@@ -217,7 +221,19 @@
     <t>CAP 100n, 50V, 0603</t>
   </si>
   <si>
-    <t>C2,C3,C27,C32, C301</t>
+    <t>C2,C3,C27,C32</t>
+  </si>
+  <si>
+    <t>GRM155R71C104KA88D</t>
+  </si>
+  <si>
+    <t>81-GRM155R71C104KA88</t>
+  </si>
+  <si>
+    <t>CAP 100n, 16V, 0402</t>
+  </si>
+  <si>
+    <t>C301</t>
   </si>
   <si>
     <t>C0805C224K5RACTU</t>
@@ -400,7 +416,7 @@
     <t>RC0805JR-070RL</t>
   </si>
   <si>
-    <t>71-CRCW0805-0-E3 </t>
+    <t>71-CRCW0805-0-E3</t>
   </si>
   <si>
     <t>R 0ohm, 0805</t>
@@ -556,7 +572,7 @@
     <t>RC0603FR-0722RL</t>
   </si>
   <si>
-    <t>660-RK73H1JTTD22R0F </t>
+    <t>660-RK73H1JTTD22R0F</t>
   </si>
   <si>
     <t>R 22R, 0603</t>
@@ -568,70 +584,48 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  </numFmts>
+  <fonts count="6">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -639,907 +633,953 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
-    <border>
+  <borders count="3">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1">
-      <alignment vertical="center" horizontal="left"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2">
-      <alignment vertical="center" horizontal="left"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
-      <alignment vertical="center" horizontal="left"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="3" applyFont="1" fontId="5">
-      <alignment vertical="center" horizontal="left"/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6">
-      <alignment vertical="center" horizontal="left"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="17:17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="26.29" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="29.43"/>
-    <col min="3" customWidth="1" max="3" width="23.14"/>
-    <col min="4" customWidth="1" max="4" width="7.71"/>
-    <col min="5" customWidth="1" max="5" width="45.71"/>
-    <col min="6" customWidth="1" max="6" width="28.71"/>
-    <col min="7" customWidth="1" max="7" width="11.43"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.71428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.7091836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.7091836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="26.2857142857143"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="4" r="A1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="4" r="B1">
-        <v>1</v>
-      </c>
-      <c t="s" s="4" r="C1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="4" r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="4" r="E1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="4" r="F1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" r="2" ht="12.0">
-      <c t="s" s="6" r="A2">
+    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="6" r="B2">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="6" r="C2">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c s="5" r="D2">
-        <v>1</v>
-      </c>
-      <c t="s" s="5" r="E2">
+      <c r="D2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c s="5" r="F2"/>
-    </row>
-    <row customHeight="1" r="3" ht="12.0">
-      <c t="s" s="7" r="A3">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="7" r="B3">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="7" r="C3">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c t="s" r="E3">
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" r="4" ht="12.0">
-      <c t="s" s="7" r="A4">
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="7" r="B4">
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="7" r="C4">
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c t="s" r="E4">
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>17</v>
       </c>
-      <c t="s" r="F4">
+      <c r="F4" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row customHeight="1" r="5" ht="12.0">
-      <c t="s" s="7" r="A5">
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="7" r="B5">
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="7" r="C5">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c t="s" r="E5">
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="F5">
+      <c r="F5" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row customHeight="1" r="6" ht="12.0">
-      <c t="s" s="7" r="A6">
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="7" r="B6">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="7" r="C6">
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c t="s" r="E6">
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row customHeight="1" r="7" ht="12.0">
-      <c t="s" s="7" r="A7">
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="7" r="B7">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="7" r="C7">
+      <c r="C7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c t="s" r="E7">
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row customHeight="1" r="8" ht="12.0">
-      <c t="s" s="7" r="A8">
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="7" r="B8">
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="7" r="C8">
+      <c r="C8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c t="s" r="E8">
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row customHeight="1" r="9" ht="12.0">
-      <c t="s" s="7" r="A9">
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="7" r="B9">
+      <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="7" r="C9">
+      <c r="C9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c t="s" r="E9">
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row customHeight="1" r="10" ht="12.0">
-      <c t="s" s="7" r="A10">
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="7" r="B10">
+      <c r="B10" s="4" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="7" r="C10">
+      <c r="C10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0" t="n">
         <v>6</v>
       </c>
-      <c t="s" r="E10">
+      <c r="E10" s="0" t="s">
         <v>42</v>
       </c>
     </row>
-    <row customHeight="1" r="11" ht="12.0">
-      <c t="s" s="7" r="A11">
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="7" r="B11">
+      <c r="B11" s="4" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="7" r="C11">
+      <c r="C11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="0" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="E11">
+      <c r="E11" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row customHeight="1" r="12" ht="12.0">
-      <c t="s" s="7" r="A12">
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="7" r="B12">
+      <c r="B12" s="4" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="7" r="C12">
+      <c r="C12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c t="s" r="E12">
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="7" r="F12">
+      <c r="F12" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row customHeight="1" r="13" ht="12.0">
-      <c t="s" s="7" r="A13">
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="7" r="B13">
+      <c r="B13" s="4" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="7" r="C13">
+      <c r="C13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="0" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="E13">
+      <c r="E13" s="0" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="7" r="F13">
+      <c r="F13" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row customHeight="1" r="14" ht="12.0">
-      <c t="s" s="7" r="A14">
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="7" r="B14">
+      <c r="B14" s="4" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="7" r="C14">
+      <c r="C14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0" t="n">
         <v>8</v>
       </c>
-      <c t="s" r="E14">
+      <c r="E14" s="0" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="7" r="F14">
+      <c r="F14" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row customHeight="1" r="15" ht="12.0">
-      <c t="s" s="7" r="A15">
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="7" r="B15">
+      <c r="B15" s="4" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="7" r="C15">
+      <c r="C15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="0" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="E15">
+      <c r="E15" s="0" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="7" r="F15">
+      <c r="F15" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row customHeight="1" r="16" ht="12.0">
-      <c t="s" s="7" r="A16">
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="7" r="B16">
+      <c r="B16" s="4" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="7" r="C16">
+      <c r="C16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c t="s" r="E16">
+      <c r="D16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="7" r="F16">
+      <c r="F16" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row customHeight="1" r="17" ht="12.0">
-      <c t="s" s="7" r="A17">
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="7" r="B17">
+      <c r="B17" s="5" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="7" r="C17">
+      <c r="C17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="0" t="n">
         <v>3</v>
       </c>
-      <c t="s" r="E17">
-        <v>72</v>
-      </c>
-      <c t="s" s="7" r="F17">
+      <c r="E18" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row customHeight="1" r="18" ht="12.0">
-      <c t="s" s="7" r="A18">
-        <v>73</v>
-      </c>
-      <c t="s" s="7" r="B18">
-        <v>74</v>
-      </c>
-      <c t="s" s="7" r="C18">
-        <v>75</v>
-      </c>
-      <c r="D18">
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="0" t="n">
         <v>11</v>
       </c>
-      <c t="s" r="E18">
-        <v>76</v>
-      </c>
-      <c t="s" s="7" r="F18">
+      <c r="E19" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row customHeight="1" r="19" ht="12.0">
-      <c t="s" s="7" r="A19">
-        <v>77</v>
-      </c>
-      <c t="s" s="7" r="B19">
-        <v>78</v>
-      </c>
-      <c t="s" s="7" r="C19">
-        <v>79</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c t="s" r="E19">
-        <v>80</v>
-      </c>
-      <c t="s" s="7" r="F19">
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" s="7" r="A20">
-        <v>81</v>
-      </c>
-      <c t="s" s="7" r="B20">
-        <v>82</v>
-      </c>
-      <c t="s" s="7" r="C20">
-        <v>83</v>
-      </c>
-      <c r="D20">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="0" t="n">
         <v>3</v>
       </c>
-      <c t="s" r="E20">
-        <v>84</v>
-      </c>
-      <c t="str" s="1" r="F20">
-        <f>HYPERLINK("http://www.ebay.com/sch/i.html?_trksid=p2054436.m570.l1313.TR0.TRC0.Xjst+6+pin+2.0&amp;_nkw=jst+6+pin+2.0&amp;_sacat=0&amp;_from=R40","Can be found on ebay")</f>
+      <c r="E21" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="6" t="str">
+        <f aca="false">HYPERLINK("http://www.ebay.com/sch/i.html?_trksid=p2054436.m570.l1313.TR0.TRC0.Xjst+6+pin+2.0&amp;_nkw=jst+6+pin+2.0&amp;_sacat=0&amp;_from=R40","Can be found on ebay")</f>
         <v>Can be found on ebay</v>
       </c>
     </row>
-    <row customHeight="1" r="21" ht="12.0">
-      <c t="s" s="7" r="A21">
-        <v>85</v>
-      </c>
-      <c t="s" s="7" r="B21">
-        <v>82</v>
-      </c>
-      <c t="s" s="7" r="C21">
+    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c t="s" r="E21">
-        <v>87</v>
-      </c>
-      <c t="str" r="F21">
-        <f>HYPERLINK("http://www.ebay.com/sch/i.html?_from=R40&amp;_trksid=p2050601.m570.l1313.TR0.TRC0.H0.Xjst+4+pin+2.0&amp;_nkw=jst+4+pin+2.0&amp;_sacat=0", "Can be found on ebay")</f>
+      <c r="C22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.ebay.com/sch/i.html?_from=R40&amp;_trksid=p2050601.m570.l1313.TR0.TRC0.H0.Xjst+4+pin+2.0&amp;_nkw=jst+4+pin+2.0&amp;_sacat=0", "Can be found on ebay")</f>
         <v>Can be found on ebay</v>
       </c>
     </row>
-    <row customHeight="1" r="22" ht="12.0">
-      <c t="s" s="7" r="A22">
-        <v>88</v>
-      </c>
-      <c t="s" s="7" r="B22">
-        <v>89</v>
-      </c>
-      <c t="s" s="7" r="C22">
-        <v>90</v>
-      </c>
-      <c r="D22">
+    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="0" t="n">
         <v>6</v>
       </c>
-      <c t="s" r="E22">
-        <v>91</v>
-      </c>
-    </row>
-    <row customHeight="1" r="23" ht="12.0">
-      <c t="s" s="7" r="A23">
-        <v>92</v>
-      </c>
-      <c t="s" s="7" r="B23">
-        <v>93</v>
-      </c>
-      <c t="s" s="7" r="C23">
-        <v>94</v>
-      </c>
-      <c r="D23">
+      <c r="E23" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="0" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="E23">
-        <v>95</v>
-      </c>
-    </row>
-    <row customHeight="1" r="24" ht="12.0">
-      <c t="s" s="7" r="A24">
-        <v>96</v>
-      </c>
-      <c t="s" s="7" r="B24">
-        <v>97</v>
-      </c>
-      <c t="s" s="7" r="C24">
-        <v>98</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c t="s" r="E24">
+      <c r="E24" s="0" t="s">
         <v>99</v>
       </c>
     </row>
-    <row customHeight="1" r="25" ht="12.0">
-      <c t="s" s="7" r="A25">
+    <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="7" r="B25">
+      <c r="B25" s="4" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="7" r="C25">
+      <c r="C25" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="0" t="n">
         <v>4</v>
       </c>
-      <c t="s" r="E25">
-        <v>103</v>
-      </c>
-    </row>
-    <row customHeight="1" r="26" ht="12.0">
-      <c t="s" s="7" r="A26">
-        <v>104</v>
-      </c>
-      <c t="s" s="7" r="B26">
-        <v>105</v>
-      </c>
-      <c t="s" s="7" r="C26">
-        <v>106</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c t="s" r="E26">
+      <c r="E26" s="0" t="s">
         <v>107</v>
       </c>
     </row>
-    <row customHeight="1" r="27" ht="12.0">
-      <c t="s" s="7" r="A27">
+    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="7" r="B27">
+      <c r="B27" s="4" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="7" r="C27">
+      <c r="C27" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c t="s" r="E27">
+      <c r="D27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row customHeight="1" r="28" ht="12.0">
-      <c t="s" s="7" r="A28">
+    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>112</v>
       </c>
-      <c t="s" s="7" r="B28">
+      <c r="B28" s="4" t="s">
         <v>113</v>
       </c>
-      <c t="s" s="7" r="C28">
+      <c r="C28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c t="s" r="E28">
+      <c r="D28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>115</v>
       </c>
     </row>
-    <row customHeight="1" r="29" ht="12.0">
-      <c t="s" r="A29">
+    <row r="29" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>116</v>
       </c>
-      <c t="s" r="B29">
+      <c r="B29" s="4" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="7" r="C29">
+      <c r="C29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c t="s" r="E29">
+      <c r="D29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>119</v>
       </c>
     </row>
-    <row customHeight="1" r="30" ht="12.0">
-      <c t="s" r="A30">
+    <row r="30" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>120</v>
       </c>
-      <c t="s" r="B30">
+      <c r="B30" s="0" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="7" r="C30">
+      <c r="C30" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c t="s" r="E30">
+      <c r="D30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>123</v>
       </c>
     </row>
-    <row customHeight="1" r="31" ht="12.0">
-      <c t="s" r="A31">
+    <row r="31" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>124</v>
       </c>
-      <c t="s" r="B31">
+      <c r="B31" s="0" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="7" r="C31">
+      <c r="C31" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c t="s" r="E31">
+      <c r="D31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>127</v>
       </c>
     </row>
-    <row customHeight="1" r="32" ht="12.0">
-      <c t="s" r="A32">
+    <row r="32" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>128</v>
       </c>
-      <c t="s" r="B32">
+      <c r="B32" s="0" t="s">
         <v>129</v>
       </c>
-      <c t="s" s="7" r="C32">
+      <c r="C32" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c t="s" r="E32">
+      <c r="D32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>131</v>
       </c>
     </row>
-    <row customHeight="1" r="33" ht="12.0">
-      <c t="s" s="7" r="A33">
+    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="7" r="B33">
+      <c r="B33" s="0" t="s">
         <v>133</v>
       </c>
-      <c t="s" s="7" r="C33">
+      <c r="C33" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c t="s" r="E33">
+      <c r="D33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>135</v>
       </c>
     </row>
-    <row customHeight="1" r="34" ht="12.0">
-      <c t="s" s="7" r="A34">
+    <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
-      <c t="s" s="7" r="B34">
+      <c r="B34" s="4" t="s">
         <v>137</v>
       </c>
-      <c t="s" s="7" r="C34">
+      <c r="C34" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="0" t="n">
         <v>6</v>
       </c>
-      <c t="s" r="E34">
-        <v>139</v>
-      </c>
-    </row>
-    <row customHeight="1" r="35" ht="12.0">
-      <c t="s" s="7" r="A35">
-        <v>140</v>
-      </c>
-      <c t="s" s="7" r="B35">
-        <v>141</v>
-      </c>
-      <c t="s" s="7" r="C35">
-        <v>142</v>
-      </c>
-      <c r="D35">
+      <c r="E35" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="0" t="n">
         <v>10</v>
       </c>
-      <c t="s" r="E35">
-        <v>143</v>
-      </c>
-    </row>
-    <row customHeight="1" r="36" ht="12.0">
-      <c t="s" s="7" r="A36">
-        <v>144</v>
-      </c>
-      <c t="s" s="7" r="B36">
-        <v>145</v>
-      </c>
-      <c t="s" s="7" r="C36">
-        <v>146</v>
-      </c>
-      <c r="D36">
+      <c r="E36" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="0" t="n">
         <v>8</v>
       </c>
-      <c t="s" r="E36">
-        <v>147</v>
-      </c>
-    </row>
-    <row customHeight="1" r="37" ht="12.0">
-      <c t="s" s="7" r="A37">
-        <v>148</v>
-      </c>
-      <c t="s" s="7" r="B37">
-        <v>149</v>
-      </c>
-      <c t="s" s="7" r="C37">
-        <v>150</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c t="s" r="E37">
+      <c r="E37" s="0" t="s">
         <v>151</v>
       </c>
     </row>
-    <row customHeight="1" r="38" ht="12.0">
-      <c t="s" s="7" r="A38">
+    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
         <v>152</v>
       </c>
-      <c t="s" s="7" r="B38">
+      <c r="B38" s="4" t="s">
         <v>153</v>
       </c>
-      <c t="s" s="7" r="C38">
+      <c r="C38" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="0" t="n">
         <v>9</v>
       </c>
-      <c t="s" r="E38">
-        <v>155</v>
-      </c>
-    </row>
-    <row customHeight="1" r="39" ht="12.0">
-      <c t="s" s="7" r="A39">
-        <v>156</v>
-      </c>
-      <c t="s" s="7" r="B39">
-        <v>157</v>
-      </c>
-      <c t="s" s="7" r="C39">
-        <v>158</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c t="s" r="E39">
+      <c r="E39" s="0" t="s">
         <v>159</v>
       </c>
     </row>
-    <row customHeight="1" r="40" ht="12.0">
-      <c t="s" s="7" r="A40">
+    <row r="40" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="7" r="B40">
+      <c r="B40" s="4" t="s">
         <v>161</v>
       </c>
-      <c t="s" s="7" r="C40">
+      <c r="C40" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c t="s" r="E40">
+      <c r="D40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>163</v>
       </c>
     </row>
-    <row customHeight="1" r="41" ht="12.0">
-      <c t="s" s="7" r="A41">
+    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
         <v>164</v>
       </c>
-      <c t="s" s="7" r="B41">
+      <c r="B41" s="4" t="s">
         <v>165</v>
       </c>
-      <c t="s" s="7" r="C41">
+      <c r="C41" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42" s="0" t="n">
         <v>7</v>
       </c>
-      <c t="s" r="E41">
-        <v>167</v>
-      </c>
-    </row>
-    <row customHeight="1" r="42" ht="12.0">
-      <c t="s" s="7" r="A42">
-        <v>168</v>
-      </c>
-      <c t="s" s="7" r="B42">
-        <v>169</v>
-      </c>
-      <c t="s" s="7" r="C42">
-        <v>170</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c t="s" r="E42">
+      <c r="E42" s="0" t="s">
         <v>171</v>
       </c>
     </row>
-    <row customHeight="1" r="43" ht="12.0">
-      <c t="s" s="7" r="A43">
+    <row r="43" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
         <v>172</v>
       </c>
-      <c t="s" s="7" r="B43">
+      <c r="B43" s="4" t="s">
         <v>173</v>
       </c>
-      <c t="s" s="7" r="C43">
+      <c r="C43" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c t="s" r="E43">
+      <c r="D43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>175</v>
       </c>
     </row>
-    <row customHeight="1" r="44" ht="12.0">
-      <c t="s" s="7" r="A44">
+    <row r="44" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="7" r="B44">
+      <c r="B44" s="4" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="7" r="C44">
+      <c r="C44" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c t="s" r="E44">
+      <c r="D44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>179</v>
       </c>
     </row>
-    <row customHeight="1" r="45" ht="12.0">
-      <c t="s" s="7" r="A45">
+    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="7" r="B45">
+      <c r="B45" s="4" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="7" r="C45">
+      <c r="C45" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" s="0" t="n">
         <v>2</v>
       </c>
-      <c t="s" r="E45">
-        <v>183</v>
-      </c>
-    </row>
-    <row customHeight="1" r="46" ht="12.0">
-      <c s="7" r="C46"/>
+      <c r="E46" s="0" t="s">
+        <v>187</v>
+      </c>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>